<commit_message>
update thesis overleaf chapter results
</commit_message>
<xml_diff>
--- a/thesis/graphs/wpm.xlsx
+++ b/thesis/graphs/wpm.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samii\Documents\mtd\thesis\thesisType\thesis\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4552E706-65E1-450A-ABC3-91882E26EF85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA150AA-A60B-4D3D-8B2B-B1986117E3A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="1" xr2:uid="{5BCCB96D-E4D3-4CE0-AFF7-989508396116}"/>
+    <workbookView xWindow="6270" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{5BCCB96D-E4D3-4CE0-AFF7-989508396116}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="trial" sheetId="1" r:id="rId1"/>
+    <sheet name="wpm" sheetId="2" r:id="rId2"/>
+    <sheet name="error" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>y = 2.08x^0.4732946</t>
   </si>
@@ -44,9 +45,6 @@
   </si>
   <si>
     <t>real data</t>
-  </si>
-  <si>
-    <t>wpm avg</t>
   </si>
   <si>
     <t>xy</t>
@@ -60,12 +58,33 @@
   <si>
     <t>sum</t>
   </si>
+  <si>
+    <t>error rates</t>
+  </si>
+  <si>
+    <t>phrases completed</t>
+  </si>
+  <si>
+    <t>session nr.</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>\\</t>
+  </si>
+  <si>
+    <t>fitted data</t>
+  </si>
+  <si>
+    <t>WPM average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +92,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,13 +124,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -168,7 +205,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$2</c:f>
+              <c:f>trial!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -203,7 +240,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$12</c:f>
+              <c:f>trial!$J$3:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -242,7 +279,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$12</c:f>
+              <c:f>trial!$K$3:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -291,7 +328,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$2</c:f>
+              <c:f>trial!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -326,7 +363,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$12</c:f>
+              <c:f>trial!$J$3:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -365,7 +402,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$12</c:f>
+              <c:f>trial!$L$3:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -637,11 +674,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$1</c:f>
+              <c:f>wpm!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wpm exp</c:v>
+                  <c:v>fitted data</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -660,7 +697,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$89</c:f>
+              <c:f>wpm!$A$2:$A$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
@@ -933,7 +970,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$89</c:f>
+              <c:f>wpm!$B$2:$B$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
@@ -1216,11 +1253,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$C$1</c:f>
+              <c:f>wpm!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>wpm avg</c:v>
+                  <c:v>WPM average</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1247,7 +1284,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$89</c:f>
+              <c:f>wpm!$A$2:$A$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
@@ -1520,7 +1557,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$89</c:f>
+              <c:f>wpm!$C$2:$C$89</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
@@ -2002,6 +2039,462 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>error!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>error rates</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="3175" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="3175">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>error!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>error!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15.98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A0C2-4E8A-B7A5-16E63082AD78}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="651328872"/>
+        <c:axId val="651329200"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>error!$B$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="9525" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>error!$A$2:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>16</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>32</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>56</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>88</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>error!$B$2:$B$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-A0C2-4E8A-B7A5-16E63082AD78}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="651328872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="88"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="651329200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="8"/>
+        <c:minorUnit val="2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="651329200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="651328872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.75948174825314396"/>
+          <c:y val="0.82268827710404813"/>
+          <c:w val="0.21522175247877035"/>
+          <c:h val="4.1058681533421459E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="sysDot"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2082,6 +2575,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2586,6 +3119,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3167,6 +4216,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>297651</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>438146</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B784C61A-47E2-44D0-AD61-70AC5CCAE6B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3480,13 +4572,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB892F25-D47A-438B-B7CB-EF9BDCD5D2CB}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J12"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.86328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1">
@@ -3736,7 +4832,7 @@
         <v>1.1858777727518774</v>
       </c>
     </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="14:18" x14ac:dyDescent="0.45">
       <c r="N17">
         <v>49</v>
       </c>
@@ -3751,7 +4847,7 @@
         <v>1.0190669081076</v>
       </c>
     </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="14:18" x14ac:dyDescent="0.45">
       <c r="N18">
         <v>57</v>
       </c>
@@ -3766,7 +4862,7 @@
         <v>1.235445178819045</v>
       </c>
     </row>
-    <row r="19" spans="14:17" x14ac:dyDescent="0.45">
+    <row r="19" spans="14:18" x14ac:dyDescent="0.45">
       <c r="N19">
         <v>56</v>
       </c>
@@ -3781,7 +4877,7 @@
         <v>0.75464789498011431</v>
       </c>
     </row>
-    <row r="20" spans="14:17" x14ac:dyDescent="0.45">
+    <row r="20" spans="14:18" x14ac:dyDescent="0.45">
       <c r="N20">
         <v>37</v>
       </c>
@@ -3796,16 +4892,168 @@
         <v>1.0594995020404328</v>
       </c>
     </row>
-    <row r="23" spans="14:17" x14ac:dyDescent="0.45">
-      <c r="N23">
-        <f ca="1">RANDBETWEEN(70,120)</f>
-        <v>98</v>
+    <row r="31" spans="14:18" x14ac:dyDescent="0.45">
+      <c r="O31" t="s">
+        <v>9</v>
+      </c>
+      <c r="P31" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>8</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="14:18" x14ac:dyDescent="0.45">
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q32">
+        <v>4</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O33">
+        <v>2</v>
+      </c>
+      <c r="P33" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q33">
+        <v>8</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O34">
+        <v>3</v>
+      </c>
+      <c r="P34" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q34">
+        <v>12</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O35">
+        <v>4</v>
+      </c>
+      <c r="P35" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q35">
+        <v>16</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O36">
+        <v>5</v>
+      </c>
+      <c r="P36" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q36">
+        <v>24</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O37">
+        <v>6</v>
+      </c>
+      <c r="P37" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q37">
+        <v>32</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O38">
+        <v>7</v>
+      </c>
+      <c r="P38" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q38">
+        <v>44</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O39">
+        <v>8</v>
+      </c>
+      <c r="P39" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q39">
+        <v>56</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O40">
+        <v>9</v>
+      </c>
+      <c r="P40" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q40">
+        <v>72</v>
+      </c>
+      <c r="R40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="15:18" x14ac:dyDescent="0.45">
+      <c r="O41">
+        <v>10</v>
+      </c>
+      <c r="P41" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q41">
+        <v>88</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R31" r:id="rId1" xr:uid="{548A66D2-E598-4D35-BBD5-3FD98F7390A8}"/>
+    <hyperlink ref="R32:R41" r:id="rId2" display="\\" xr:uid="{181F14B0-C131-45FC-9674-8B4EFDC24EC6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -3813,8 +5061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFA5080-83A4-48B0-9E86-96BE7C4E1BDB}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3825,19 +5073,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
@@ -5936,7 +7184,7 @@
         <v>240.82562488659607</v>
       </c>
       <c r="F68">
-        <f t="shared" ref="F68:F90" si="8">B68*B68</f>
+        <f t="shared" ref="F68:F89" si="8">B68*B68</f>
         <v>231.56310085249623</v>
       </c>
       <c r="G68">
@@ -6603,7 +7851,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B90">
         <f>SUM(B2:B89)</f>
@@ -6614,7 +7862,7 @@
         <v>1069.9282228828024</v>
       </c>
       <c r="E90">
-        <f t="shared" ref="D90:G90" si="11">SUM(E2:E89)</f>
+        <f t="shared" ref="E90:G90" si="11">SUM(E2:E89)</f>
         <v>14040.213360387505</v>
       </c>
       <c r="F90">
@@ -6650,6 +7898,237 @@
       <c r="H97">
         <f>F93/SQRT(H95)</f>
         <v>0.99223497924983128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0A059D-CF59-48AA-95DA-15F5C5D642B5}">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>15.98</v>
+      </c>
+      <c r="H2">
+        <v>109</v>
+      </c>
+      <c r="J2">
+        <v>1.1258777727518776</v>
+      </c>
+      <c r="L2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>9.25</v>
+      </c>
+      <c r="H3">
+        <v>106</v>
+      </c>
+      <c r="J3">
+        <v>1.06</v>
+      </c>
+      <c r="L3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>5.43</v>
+      </c>
+      <c r="H4">
+        <v>105</v>
+      </c>
+      <c r="J4">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>6.7</v>
+      </c>
+      <c r="H5">
+        <v>106</v>
+      </c>
+      <c r="J5">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>4.82</v>
+      </c>
+      <c r="H6">
+        <v>102</v>
+      </c>
+      <c r="J6">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>4.37</v>
+      </c>
+      <c r="H7">
+        <v>105</v>
+      </c>
+      <c r="J7">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>3.8</v>
+      </c>
+      <c r="H8">
+        <v>95</v>
+      </c>
+      <c r="J8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>5.2</v>
+      </c>
+      <c r="H9">
+        <v>95</v>
+      </c>
+      <c r="J9">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" s="1">
+        <v>72</v>
+      </c>
+      <c r="C10">
+        <v>4.93</v>
+      </c>
+      <c r="H10">
+        <v>104</v>
+      </c>
+      <c r="J10">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>88</v>
+      </c>
+      <c r="C11">
+        <v>6.57</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B2:B11)</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C2:C11)</f>
+        <v>67.05</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E2:E11)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>SUM(F2:F11)</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>SUM(G2:G11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="F15">
+        <f>(88*E12)-(B12*C12)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>(88*F12)-(B12*B12)</f>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>(88*G12)-(C12*C12)</f>
+        <v>-4495.7024999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H17">
+        <f>G15*H15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H19" t="e">
+        <f>F15/SQRT(H17)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update chapter current technology
overleaf update, update on references and wpm, changed backspace
</commit_message>
<xml_diff>
--- a/thesis/graphs/wpm.xlsx
+++ b/thesis/graphs/wpm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samii\Documents\mtd\thesis\thesisType\thesis\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD56D2C-2570-4766-9B8F-792524ECCCDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554C56C0-6ABF-483C-A99C-4D64B429C2BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="3" xr2:uid="{5BCCB96D-E4D3-4CE0-AFF7-989508396116}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="1" xr2:uid="{5BCCB96D-E4D3-4CE0-AFF7-989508396116}"/>
   </bookViews>
   <sheets>
     <sheet name="trial" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -140,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -984,268 +984,268 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
                 <c:pt idx="0">
-                  <c:v>2.08</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8876144495709739</c:v>
+                  <c:v>3.5522212117468661</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4985029815267707</c:v>
+                  <c:v>4.0827349036508807</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0088063506591718</c:v>
+                  <c:v>4.5065269775658479</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4553524301928533</c:v>
+                  <c:v>4.865311593364674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8568883467903046</c:v>
+                  <c:v>5.1795634023885562</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2244872514742031</c:v>
+                  <c:v>5.46104336197038</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5653303575458208</c:v>
+                  <c:v>5.7172074003638924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.8843861114190874</c:v>
+                  <c:v>5.9531158191032736</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.185259641998095</c:v>
+                  <c:v>6.1723796584671229</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.4706643037049192</c:v>
+                  <c:v>6.3776769440526957</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.7427023894925791</c:v>
+                  <c:v>6.5710553519829995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.0030416343583894</c:v>
+                  <c:v>6.7541199447283047</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.2530311918058894</c:v>
+                  <c:v>6.9281550245216437</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.4937806542222294</c:v>
+                  <c:v>7.0942062354882998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.7262155562910122</c:v>
+                  <c:v>7.2531376426888494</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.9511173829395085</c:v>
+                  <c:v>7.4056724869061972</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.1691530587444738</c:v>
+                  <c:v>7.5524229602158828</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.3808971109954644</c:v>
+                  <c:v>7.6939123999108485</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.5868486137412887</c:v>
+                  <c:v>7.8305921249149231</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.7874443395341828</c:v>
+                  <c:v>7.9628544086669377</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.983069106587223</c:v>
+                  <c:v>8.0910426151188997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.1740640188608555</c:v>
+                  <c:v>8.2154592177933434</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.360733100507451</c:v>
+                  <c:v>8.3363722160274225</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.5433486909737315</c:v>
+                  <c:v>8.4540203216173957</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.7221558722694272</c:v>
+                  <c:v>8.5686171908380224</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.8973761323338429</c:v>
+                  <c:v>8.6803549071889776</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.069210419542145</c:v>
+                  <c:v>8.7894068701344334</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10.237841707543112</c:v>
+                  <c:v>8.895930208572203</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10.403437163003625</c:v>
+                  <c:v>9.0000678107887229</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10.566149988847576</c:v>
+                  <c:v>9.1019500424953552</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>10.726121000406712</c:v>
+                  <c:v>9.2016962093139263</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>10.883479980274279</c:v>
+                  <c:v>9.2994158084619372</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.038346848659168</c:v>
+                  <c:v>9.3952096054422736</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11.190832679022678</c:v>
+                  <c:v>9.4891705645934614</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11.341040583263204</c:v>
+                  <c:v>9.5813846569153274</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11.489066486343532</c:v>
+                  <c:v>9.6719315642912758</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.634999806768336</c:v>
+                  <c:v>9.7608852958162693</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>11.778924056518717</c:v>
+                  <c:v>9.848314729209573</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.92091737178742</c:v>
+                  <c:v>9.9342840880931291</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>12.061052984018335</c:v>
+                  <c:v>10.018853364135861</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12.199399639249794</c:v>
+                  <c:v>10.102078691613837</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>12.336021972525179</c:v>
+                  <c:v>10.184012680748173</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>12.470980843113404</c:v>
+                  <c:v>10.264704715204712</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>12.604333635434662</c:v>
+                  <c:v>10.344201218330644</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>12.736134529880655</c:v>
+                  <c:v>10.422545892031014</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>12.866434747127142</c:v>
+                  <c:v>10.499779931627018</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>12.995282769039722</c:v>
+                  <c:v>10.575942219567802</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>13.122724538854074</c:v>
+                  <c:v>10.651069500471698</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13.248803642956723</c:v>
+                  <c:v>10.725196539638706</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>13.373561476289998</c:v>
+                  <c:v>10.798356266892483</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>13.497037393147355</c:v>
+                  <c:v>10.870579907369168</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>13.619268844904353</c:v>
+                  <c:v>10.94189710066445</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>13.740291506041386</c:v>
+                  <c:v>11.012336009574176</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>13.860139389650893</c:v>
+                  <c:v>11.081923419512202</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>13.978844953481019</c:v>
+                  <c:v>11.150684829558992</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>14.096439197445546</c:v>
+                  <c:v>11.218644535981548</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>14.212951753423965</c:v>
+                  <c:v>11.285825708967824</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>14.328410968083151</c:v>
+                  <c:v>11.35225046323372</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>14.442843979371592</c:v>
+                  <c:v>11.417939923087099</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>14.556276787266684</c:v>
+                  <c:v>11.482914282468647</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>14.668734319293485</c:v>
+                  <c:v>11.547192860432963</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>14.780240491279267</c:v>
+                  <c:v>11.610794152483853</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>14.89081826376014</c:v>
+                  <c:v>11.673735878134163</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>15.000489694413639</c:v>
+                  <c:v>11.736035025022213</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>15.109275986854044</c:v>
+                  <c:v>11.797707889883082</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>15.217197536093702</c:v>
+                  <c:v>11.858770116642992</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>15.324273970944441</c:v>
+                  <c:v>11.919236731878554</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>15.430524193606809</c:v>
+                  <c:v>11.97912217785902</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>15.535966416671609</c:v>
+                  <c:v>12.038440343368887</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>15.64061819773721</c:v>
+                  <c:v>12.097204592489296</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>15.744496471827718</c:v>
+                  <c:v>12.155427791500214</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>15.84761758178008</c:v>
+                  <c:v>12.213122334050334</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>15.949997306753463</c:v>
+                  <c:v>12.270300164728402</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>16.051650889000577</c:v>
+                  <c:v>12.326972801157565</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>16.152593059028717</c:v>
+                  <c:v>12.383151354723799</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>16.252838059267091</c:v>
+                  <c:v>12.438846550039468</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>16.352399666347399</c:v>
+                  <c:v>12.494068743234765</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>16.451291212095569</c:v>
+                  <c:v>12.548827939161528</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>16.549525603324515</c:v>
+                  <c:v>12.603133807587065</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>16.647115340510503</c:v>
+                  <c:v>12.656995698449162</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>16.744072535429062</c:v>
+                  <c:v>12.710422656237448</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>16.840408927820356</c:v>
+                  <c:v>12.763423433561329</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>16.936135901148376</c:v>
+                  <c:v>12.816006503959533</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>17.031264497513551</c:v>
+                  <c:v>12.868180074002332</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>17.125805431773422</c:v>
+                  <c:v>12.919952094733114</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>17.219769104922449</c:v>
+                  <c:v>12.971330272492855</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>17.313165616777439</c:v>
+                  <c:v>13.022322079167235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1571,268 +1571,268 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="88"/>
                 <c:pt idx="0">
-                  <c:v>2.2464000000000004</c:v>
+                  <c:v>3.024</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1763758945280713</c:v>
+                  <c:v>3.9074433329215532</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6734281306031096</c:v>
+                  <c:v>4.2868716488334249</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.513425965473731</c:v>
+                  <c:v>5.0737985563480876</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8563341489102108</c:v>
+                  <c:v>5.8383739120376088</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2454394145335295</c:v>
+                  <c:v>5.5939284745796414</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.694691104106882</c:v>
+                  <c:v>5.9525372645477148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.8992501789985701</c:v>
+                  <c:v>5.4313470303456972</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.3551370003326149</c:v>
+                  <c:v>6.4293650846315362</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.7419330097779238</c:v>
+                  <c:v>6.7278938277291642</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.8589041619272146</c:v>
+                  <c:v>6.7603375606958576</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.0798375089672083</c:v>
+                  <c:v>6.8996081195821501</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.7033457977942295</c:v>
+                  <c:v>7.4295319392011354</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.8332736871503608</c:v>
+                  <c:v>7.482407426483376</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.8684696869333415</c:v>
+                  <c:v>7.1013004417237875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.1897884896684729</c:v>
+                  <c:v>7.688325901250181</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.7462291212334602</c:v>
+                  <c:v>8.1462397355968168</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.9043768340314777</c:v>
+                  <c:v>8.232141026635313</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.9675599087651481</c:v>
+                  <c:v>8.2324862679046085</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.1879280167031787</c:v>
+                  <c:v>8.3787335736589679</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.4904398866969188</c:v>
+                  <c:v>8.5998827613602931</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.3423918708507117</c:v>
+                  <c:v>8.4146843197236567</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.5410265796152895</c:v>
+                  <c:v>8.5440775865050771</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.5479477625175999</c:v>
+                  <c:v>8.5030996603479707</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.9250826386126807</c:v>
+                  <c:v>8.7921811344820924</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10.01382054843751</c:v>
+                  <c:v>8.3115586751128809</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>10.392244938950535</c:v>
+                  <c:v>9.1143726525484272</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.572670940519252</c:v>
+                  <c:v>9.2288772136411552</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10.544976958769405</c:v>
+                  <c:v>9.1628081148293692</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>10.819574649523771</c:v>
+                  <c:v>9.3600705232202728</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10.566149988847576</c:v>
+                  <c:v>9.1019500424953552</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11.262427050427048</c:v>
+                  <c:v>9.6617810197796228</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>11.209984379682508</c:v>
+                  <c:v>9.5783982827157956</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>11.369497254118944</c:v>
+                  <c:v>9.6770658936055423</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11.414649332603132</c:v>
+                  <c:v>9.6789539758853316</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>11.681271800761101</c:v>
+                  <c:v>9.8688261966227877</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>11.489066486343532</c:v>
+                  <c:v>9.6719315642912758</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.984049800971386</c:v>
+                  <c:v>10.053711854690757</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>12.367870259344652</c:v>
+                  <c:v>10.340730465670052</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>12.397754066658917</c:v>
+                  <c:v>10.331655451616856</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.699221394497785</c:v>
+                  <c:v>9.7182877632117854</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.955411646464798</c:v>
+                  <c:v>9.9000371177815598</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11.719220873898919</c:v>
+                  <c:v>9.3692916662883192</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>11.847431800957732</c:v>
+                  <c:v>9.7514694794444754</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>11.974116953662929</c:v>
+                  <c:v>9.8269911574141116</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>12.099327803386622</c:v>
+                  <c:v>10.318320433110703</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>12.73777039965587</c:v>
+                  <c:v>10.394782132310747</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>12.865329941349325</c:v>
+                  <c:v>10.470182797372123</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>12.59781555729991</c:v>
+                  <c:v>10.22502672045283</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>12.983827570097588</c:v>
+                  <c:v>10.510692608845931</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>12.838619017238397</c:v>
+                  <c:v>10.366422016216784</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>13.497037393147355</c:v>
+                  <c:v>10.870579907369168</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>12.938305402659134</c:v>
+                  <c:v>10.394802245631228</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>13.328082760860143</c:v>
+                  <c:v>10.68196592928695</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>13.444335207961366</c:v>
+                  <c:v>10.749465716926837</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>13.279902705806968</c:v>
+                  <c:v>10.593150588081041</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>13.814510413496635</c:v>
+                  <c:v>10.994271645261918</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>13.502304165752767</c:v>
+                  <c:v>10.721534423519433</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>13.611990419678992</c:v>
+                  <c:v>10.784637940072033</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>13.865130220196727</c:v>
+                  <c:v>10.961222326163615</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>14.410714019394018</c:v>
+                  <c:v>11.368085139643961</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>15.40217103525816</c:v>
+                  <c:v>12.124552503454611</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>15.519252515843231</c:v>
+                  <c:v>12.191333860108047</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>15.486450994310546</c:v>
+                  <c:v>12.14068531325953</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>15.600509282190185</c:v>
+                  <c:v>11.618674674771992</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>15.713647026328207</c:v>
+                  <c:v>12.269616205478405</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>15.825885437537449</c:v>
+                  <c:v>12.333120921308712</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>15.784002190072774</c:v>
+                  <c:v>12.276813833834911</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>16.202050403287149</c:v>
+                  <c:v>12.817660730309152</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>16.157405073338474</c:v>
+                  <c:v>12.519977957103643</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>16.422649107624071</c:v>
+                  <c:v>12.702064822113762</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>16.374276330700827</c:v>
+                  <c:v>12.641644903160223</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>16.639998460869084</c:v>
+                  <c:v>12.823778450752851</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>16.587997199023601</c:v>
+                  <c:v>12.761112171317539</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>16.533200415670596</c:v>
+                  <c:v>12.696781985192292</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>16.798696781389868</c:v>
+                  <c:v>12.395534506078521</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>16.740423201045104</c:v>
+                  <c:v>12.812011946540652</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>17.333543646328245</c:v>
+                  <c:v>13.243712867828851</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>17.438368684821302</c:v>
+                  <c:v>12.799804497944759</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>17.542497139523988</c:v>
+                  <c:v>13.359321836042289</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>17.645942260941133</c:v>
+                  <c:v>13.28984548337162</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>17.748716887554806</c:v>
+                  <c:v>13.473048015611695</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>18.01923755276778</c:v>
+                  <c:v>13.273960370903783</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>17.782942696205794</c:v>
+                  <c:v>12.687846438919937</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>18.223453012339501</c:v>
+                  <c:v>13.254225476222402</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>18.153353757679827</c:v>
+                  <c:v>13.178351136627777</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>18.252955251217795</c:v>
+                  <c:v>13.101043575217783</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>17.313165616777439</c:v>
+                  <c:v>13.022322079167235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5070,8 +5070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFA5080-83A4-48B0-9E86-96BE7C4E1BDB}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5102,24 +5102,24 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B4" si="0">2.08*POWER(A2,0.4732946)</f>
-        <v>2.08</v>
+        <f>2.8*POWER(A2,0.3432946)</f>
+        <v>2.8</v>
       </c>
       <c r="C2">
         <f>B2*J2</f>
-        <v>2.2464000000000004</v>
+        <v>3.024</v>
       </c>
       <c r="E2">
         <f>B2*C2</f>
-        <v>4.6725120000000011</v>
+        <v>8.4672000000000001</v>
       </c>
       <c r="F2">
         <f>B2*B2</f>
-        <v>4.3264000000000005</v>
+        <v>7.839999999999999</v>
       </c>
       <c r="G2">
         <f>C2*C2</f>
-        <v>5.0463129600000016</v>
+        <v>9.1445760000000007</v>
       </c>
       <c r="H2">
         <v>108</v>
@@ -5136,24 +5136,24 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" si="0"/>
-        <v>2.8876144495709739</v>
+        <f t="shared" ref="B3:B66" si="0">2.8*POWER(A3,0.3432946)</f>
+        <v>3.5522212117468661</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" si="1">B3*J3</f>
-        <v>3.1763758945280713</v>
+        <v>3.9074433329215532</v>
       </c>
       <c r="E3">
         <f>B3*C3</f>
-        <v>9.172148930308186</v>
+        <v>13.880103090902812</v>
       </c>
       <c r="F3">
         <f>B3*B3</f>
-        <v>8.3383172093710787</v>
+        <v>12.618275537184374</v>
       </c>
       <c r="G3">
         <f>C3*C3</f>
-        <v>10.089363823339005</v>
+        <v>15.268113399993096</v>
       </c>
       <c r="H3">
         <v>110</v>
@@ -5171,23 +5171,23 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>3.4985029815267707</v>
+        <v>4.0827349036508807</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
-        <v>3.6734281306031096</v>
+        <v>4.2868716488334249</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E67" si="2">B4*C4</f>
-        <v>12.851499267339291</v>
+        <v>17.502160508163623</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F67" si="3">B4*B4</f>
-        <v>12.239523111751705</v>
+        <v>16.668724293489166</v>
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G67" si="4">C4*C4</f>
-        <v>13.494074230706257</v>
+        <v>18.377268533571808</v>
       </c>
       <c r="H4">
         <v>105</v>
@@ -5204,24 +5204,24 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f>2.08*POWER(A5,0.4732946)</f>
-        <v>4.0088063506591718</v>
+        <f t="shared" si="0"/>
+        <v>4.5065269775658479</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>4.513425965473731</v>
+        <v>5.0737985563480876</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>18.093450673621096</v>
+        <v>22.865210072917311</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>16.070528357085308</v>
+        <v>20.308785399528777</v>
       </c>
       <c r="G5">
         <f t="shared" si="4"/>
-        <v>20.371013945812482</v>
+        <v>25.743431790399939</v>
       </c>
       <c r="H5">
         <v>109</v>
@@ -5241,30 +5241,30 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <f t="shared" ref="B6:B69" si="5">2.08*POWER(A6,0.4732946)</f>
-        <v>4.4553524301928533</v>
+        <f t="shared" si="0"/>
+        <v>4.865311593364674</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>4.8563341489102108</v>
+        <v>5.8383739120376088</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>21.63668015217565</v>
+        <v>28.405508280634443</v>
       </c>
       <c r="F6">
         <f t="shared" si="3"/>
-        <v>19.850165277225365</v>
+        <v>23.671256900528704</v>
       </c>
       <c r="G6">
         <f t="shared" si="4"/>
-        <v>23.583981365871463</v>
+        <v>34.086609936761334</v>
       </c>
       <c r="H6">
         <v>109</v>
       </c>
       <c r="J6">
-        <v>1.0900000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="L6">
         <v>24</v>
@@ -5275,24 +5275,24 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" si="5"/>
-        <v>4.8568883467903046</v>
+        <f t="shared" si="0"/>
+        <v>5.1795634023885562</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>5.2454394145335295</v>
+        <v>5.5939284745796414</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>25.476513566242456</v>
+        <v>28.974107202511952</v>
       </c>
       <c r="F7">
         <f t="shared" si="3"/>
-        <v>23.589364413187457</v>
+        <v>26.827877039362917</v>
       </c>
       <c r="G7">
         <f t="shared" si="4"/>
-        <v>27.514634651541858</v>
+        <v>31.292035778712915</v>
       </c>
       <c r="H7">
         <v>108</v>
@@ -5309,24 +5309,24 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" si="5"/>
-        <v>5.2244872514742031</v>
+        <f t="shared" si="0"/>
+        <v>5.46104336197038</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>5.694691104106882</v>
+        <v>5.9525372645477148</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>29.75184107448996</v>
+        <v>32.507064115439618</v>
       </c>
       <c r="F8">
         <f t="shared" si="3"/>
-        <v>27.295267040816473</v>
+        <v>29.822994601320751</v>
       </c>
       <c r="G8">
         <f t="shared" si="4"/>
-        <v>32.429506771194056</v>
+        <v>35.432699885829194</v>
       </c>
       <c r="H8">
         <v>109</v>
@@ -5343,30 +5343,30 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" si="5"/>
-        <v>5.5653303575458208</v>
+        <f t="shared" si="0"/>
+        <v>5.7172074003638924</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>5.8992501789985701</v>
+        <v>5.4313470303456972</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>32.831276107938358</v>
+        <v>31.052137435836869</v>
       </c>
       <c r="F9">
         <f t="shared" si="3"/>
-        <v>30.972901988621093</v>
+        <v>32.686460458775656</v>
       </c>
       <c r="G9">
         <f t="shared" si="4"/>
-        <v>34.801152674414659</v>
+        <v>29.499530564045024</v>
       </c>
       <c r="H9">
         <v>106</v>
       </c>
       <c r="J9">
-        <v>1.06</v>
+        <v>0.95</v>
       </c>
       <c r="L9">
         <v>56</v>
@@ -5377,24 +5377,24 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" si="5"/>
-        <v>5.8843861114190874</v>
+        <f t="shared" si="0"/>
+        <v>5.9531158191032736</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>6.3551370003326149</v>
+        <v>6.4293650846315362</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>37.3960799009228</v>
+        <v>38.274754992110253</v>
       </c>
       <c r="F10">
         <f t="shared" si="3"/>
-        <v>34.625999908261846</v>
+        <v>35.439587955657643</v>
       </c>
       <c r="G10">
         <f t="shared" si="4"/>
-        <v>40.387766292996623</v>
+        <v>41.336735391479081</v>
       </c>
       <c r="H10">
         <v>108</v>
@@ -5411,24 +5411,24 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" si="5"/>
-        <v>6.185259641998095</v>
+        <f t="shared" si="0"/>
+        <v>6.1723796584671229</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>6.7419330097779238</v>
+        <v>6.7278938277291642</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>41.700606154434141</v>
+        <v>41.527115006602003</v>
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>38.257436838930403</v>
+        <v>38.098270648258719</v>
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>45.453660708333217</v>
+        <v>45.264555357196187</v>
       </c>
       <c r="H11">
         <v>109</v>
@@ -5445,24 +5445,24 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" si="5"/>
-        <v>6.4706643037049192</v>
+        <f t="shared" si="0"/>
+        <v>6.3776769440526957</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>6.8589041619272146</v>
+        <v>6.7603375606958576</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>44.381666323115532</v>
+        <v>43.115248994863414</v>
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>41.869496531241069</v>
+        <v>40.674763202701328</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>47.044566302502467</v>
+        <v>45.702163934555216</v>
       </c>
       <c r="H12">
         <v>106</v>
@@ -5476,24 +5476,24 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" si="5"/>
-        <v>6.7427023894925791</v>
+        <f t="shared" si="0"/>
+        <v>6.5710553519829995</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>7.0798375089672083</v>
+        <v>6.8996081195821501</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>47.737237288932384</v>
+        <v>45.33770686076565</v>
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>45.464035513268932</v>
+        <v>43.17876843882442</v>
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>50.124099153379007</v>
+        <v>47.604592203803932</v>
       </c>
       <c r="H13">
         <v>105</v>
@@ -5507,24 +5507,24 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" si="5"/>
-        <v>7.0030416343583894</v>
+        <f t="shared" si="0"/>
+        <v>6.7541199447283047</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>7.7033457977942295</v>
+        <v>7.4295319392011354</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>53.946851345812732</v>
+        <v>50.179949850554344</v>
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>49.042592132557026</v>
+        <v>45.618136227776681</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>59.341536480394012</v>
+        <v>55.197944835609782</v>
       </c>
       <c r="H14">
         <v>110</v>
@@ -5538,24 +5538,24 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" si="5"/>
-        <v>7.2530311918058894</v>
+        <f t="shared" si="0"/>
+        <v>6.9281550245216437</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>7.8332736871503608</v>
+        <v>7.482407426483376</v>
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>56.814978386853895</v>
+        <v>51.839278607308863</v>
       </c>
       <c r="F15">
         <f t="shared" si="3"/>
-        <v>52.60646146930916</v>
+        <v>47.9993320438045</v>
       </c>
       <c r="G15">
         <f t="shared" si="4"/>
-        <v>61.360176657802207</v>
+        <v>55.986420895893581</v>
       </c>
       <c r="H15">
         <v>108</v>
@@ -5569,30 +5569,30 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" si="5"/>
-        <v>7.4937806542222294</v>
+        <f t="shared" si="0"/>
+        <v>7.0942062354882998</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>7.8684696869333415</v>
+        <v>7.1013004417237875</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>58.96458591827512</v>
+        <v>50.378089873752714</v>
       </c>
       <c r="F16">
         <f t="shared" si="3"/>
-        <v>56.156748493595344</v>
+        <v>50.327762111641071</v>
       </c>
       <c r="G16">
         <f t="shared" si="4"/>
-        <v>61.912815214188875</v>
+        <v>50.42846796362646</v>
       </c>
       <c r="H16">
         <v>105</v>
       </c>
       <c r="J16">
-        <v>1.05</v>
+        <v>1.0009999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
@@ -5600,24 +5600,24 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" si="5"/>
-        <v>7.7262155562910122</v>
+        <f t="shared" si="0"/>
+        <v>7.2531376426888494</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>8.1897884896684729</v>
+        <v>7.688325901250181</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>63.276071231609627</v>
+        <v>55.764486003617364</v>
       </c>
       <c r="F17">
         <f t="shared" si="3"/>
-        <v>59.694406822273237</v>
+        <v>52.60800566378996</v>
       </c>
       <c r="G17">
         <f t="shared" si="4"/>
-        <v>67.072635505506213</v>
+        <v>59.110355163834406</v>
       </c>
       <c r="H17">
         <v>106</v>
@@ -5631,24 +5631,24 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" si="5"/>
-        <v>7.9511173829395085</v>
+        <f t="shared" si="0"/>
+        <v>7.4056724869061972</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>8.7462291212334602</v>
+        <v>8.1462397355968168</v>
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>69.542294401011105</v>
+        <v>60.328383481651358</v>
       </c>
       <c r="F18">
         <f t="shared" si="3"/>
-        <v>63.220267637282817</v>
+        <v>54.843984983319416</v>
       </c>
       <c r="G18">
         <f t="shared" si="4"/>
-        <v>76.496523841112221</v>
+        <v>66.3612218298165</v>
       </c>
       <c r="H18">
         <v>110</v>
@@ -5662,24 +5662,24 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" si="5"/>
-        <v>8.1691530587444738</v>
+        <f t="shared" si="0"/>
+        <v>7.5524229602158828</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>8.9043768340314777</v>
+        <v>8.232141026635313</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>72.741217249941684</v>
+        <v>62.172610901295684</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
-        <v>66.735061697194197</v>
+        <v>57.039092569996036</v>
       </c>
       <c r="G19">
         <f t="shared" si="4"/>
-        <v>79.287926802436445</v>
+        <v>67.768145882412298</v>
       </c>
       <c r="H19">
         <v>109</v>
@@ -5693,24 +5693,24 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" si="5"/>
-        <v>8.3808971109954644</v>
+        <f t="shared" si="0"/>
+        <v>7.6939123999108485</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>8.9675599087651481</v>
+        <v>8.2324862679046085</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>75.156196932048573</v>
+        <v>63.340028178727053</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>70.23943638509212</v>
+        <v>59.196288017501914</v>
       </c>
       <c r="G20">
         <f t="shared" si="4"/>
-        <v>80.417130717291997</v>
+        <v>67.773830151237945</v>
       </c>
       <c r="H20">
         <v>107</v>
@@ -5724,24 +5724,24 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" si="5"/>
-        <v>8.5868486137412887</v>
+        <f t="shared" si="0"/>
+        <v>7.8305921249149231</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>9.1879280167031787</v>
+        <v>8.3787335736589679</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>78.895346953382443</v>
+        <v>65.610445138654185</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>73.733969115310686</v>
+        <v>61.318173026779611</v>
       </c>
       <c r="G21">
         <f t="shared" si="4"/>
-        <v>84.418021240119202</v>
+        <v>70.203176298359978</v>
       </c>
       <c r="H21">
         <v>107</v>
@@ -5755,24 +5755,24 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" si="5"/>
-        <v>8.7874443395341828</v>
+        <f t="shared" si="0"/>
+        <v>7.9628544086669377</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>9.4904398866969188</v>
+        <v>8.5998827613602931</v>
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>83.396712262044275</v>
+        <v>68.479614360316603</v>
       </c>
       <c r="F22">
         <f t="shared" si="3"/>
-        <v>77.219178020411348</v>
+        <v>63.407050333626486</v>
       </c>
       <c r="G22">
         <f t="shared" si="4"/>
-        <v>90.068449243007819</v>
+        <v>73.95798350914194</v>
       </c>
       <c r="H22">
         <v>108</v>
@@ -5786,24 +5786,24 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" si="5"/>
-        <v>8.983069106587223</v>
+        <f t="shared" si="0"/>
+        <v>8.0910426151188997</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>9.3423918708507117</v>
+        <v>8.4146843197236567</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>83.923351796670644</v>
+        <v>68.083569423656897</v>
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>80.695530573721769</v>
+        <v>65.464970599670082</v>
       </c>
       <c r="G23">
         <f t="shared" si="4"/>
-        <v>87.280285868537462</v>
+        <v>70.806912200603179</v>
       </c>
       <c r="H23">
         <v>104</v>
@@ -5817,24 +5817,24 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" si="5"/>
-        <v>9.1740640188608555</v>
+        <f t="shared" si="0"/>
+        <v>8.2154592177933434</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>9.5410265796152895</v>
+        <v>8.5440775865050771</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>87.52998864704368</v>
+        <v>70.193520965594644</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
-        <v>84.163450622157399</v>
+        <v>67.493770159225619</v>
       </c>
       <c r="G24">
         <f t="shared" si="4"/>
-        <v>91.031188192925427</v>
+        <v>73.00126180421843</v>
       </c>
       <c r="H24">
         <v>104</v>
@@ -5848,24 +5848,24 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" si="5"/>
-        <v>9.360733100507451</v>
+        <f t="shared" si="0"/>
+        <v>8.3363722160274225</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>9.5479477625175999</v>
+        <v>8.5030996603479707</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>89.375790662514547</v>
+        <v>70.885003758637041</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>87.623324178935832</v>
+        <v>69.495101724153955</v>
       </c>
       <c r="G25">
         <f t="shared" si="4"/>
-        <v>91.163306475764841</v>
+        <v>72.302703833809773</v>
       </c>
       <c r="H25">
         <v>102</v>
@@ -5879,24 +5879,24 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <f t="shared" si="5"/>
-        <v>9.5433486909737315</v>
+        <f t="shared" si="0"/>
+        <v>8.4540203216173957</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>9.9250826386126807</v>
+        <v>8.7921811344820924</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>94.718524407010435</v>
+        <v>74.329277982252691</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>91.075504237510032</v>
+        <v>71.470459598319891</v>
       </c>
       <c r="G26">
         <f t="shared" si="4"/>
-        <v>98.507265383290857</v>
+        <v>77.30244910154282</v>
       </c>
       <c r="H26">
         <v>104</v>
@@ -5910,30 +5910,30 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <f t="shared" si="5"/>
-        <v>9.7221558722694272</v>
+        <f t="shared" si="0"/>
+        <v>8.5686171908380224</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>10.01382054843751</v>
+        <v>8.3115586751128809</v>
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
-        <v>97.355924248843991</v>
+        <v>71.218564546231136</v>
       </c>
       <c r="F27">
         <f t="shared" si="3"/>
-        <v>94.520314804702906</v>
+        <v>73.421200563124884</v>
       </c>
       <c r="G27">
         <f t="shared" si="4"/>
-        <v>100.27660197630931</v>
+        <v>69.082007609844183</v>
       </c>
       <c r="H27">
         <v>103</v>
       </c>
       <c r="J27">
-        <v>1.03</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
@@ -5941,24 +5941,24 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <f t="shared" si="5"/>
-        <v>9.8973761323338429</v>
+        <f t="shared" si="0"/>
+        <v>8.6803549071889776</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>10.392244938950535</v>
+        <v>9.1143726525484272</v>
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
-        <v>102.8559570201362</v>
+        <v>79.115989380497766</v>
       </c>
       <c r="F28">
         <f t="shared" si="3"/>
-        <v>97.958054304891618</v>
+        <v>75.348561314759763</v>
       </c>
       <c r="G28">
         <f t="shared" si="4"/>
-        <v>107.99875487114301</v>
+        <v>83.071788849522648</v>
       </c>
       <c r="H28">
         <v>105</v>
@@ -5972,24 +5972,24 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <f t="shared" si="5"/>
-        <v>10.069210419542145</v>
+        <f>2.8*POWER(A29,0.3432946)</f>
+        <v>8.7894068701344334</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>10.572670940519252</v>
+        <v>9.2288772136411552</v>
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
-        <v>106.45844839666691</v>
+        <v>81.116356785204701</v>
       </c>
       <c r="F29">
         <f t="shared" si="3"/>
-        <v>101.3889984730161</v>
+        <v>77.25367312876638</v>
       </c>
       <c r="G29">
         <f t="shared" si="4"/>
-        <v>111.78137081650026</v>
+        <v>85.17217462446493</v>
       </c>
       <c r="H29">
         <v>105</v>
@@ -6003,24 +6003,24 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <f t="shared" si="5"/>
-        <v>10.237841707543112</v>
+        <f t="shared" si="0"/>
+        <v>8.895930208572203</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>10.544976958769405</v>
+        <v>9.1628081148293692</v>
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
-        <v>107.95780491357054</v>
+        <v>81.511701504061108</v>
       </c>
       <c r="F30">
         <f t="shared" si="3"/>
-        <v>104.81340282870926</v>
+        <v>79.137574275787472</v>
       </c>
       <c r="G30">
         <f t="shared" si="4"/>
-        <v>111.19653906097766</v>
+        <v>83.957052549182933</v>
       </c>
       <c r="H30">
         <v>103</v>
@@ -6034,24 +6034,24 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <f t="shared" si="5"/>
-        <v>10.403437163003625</v>
+        <f t="shared" si="0"/>
+        <v>9.0000678107887229</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>10.819574649523771</v>
+        <v>9.3600705232202728</v>
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
-        <v>112.56076499674752</v>
+        <v>84.241269422747138</v>
       </c>
       <c r="F31">
         <f t="shared" si="3"/>
-        <v>108.23150480456492</v>
+        <v>81.001220598795314</v>
       </c>
       <c r="G31">
         <f t="shared" si="4"/>
-        <v>117.06319559661743</v>
+        <v>87.610920199657031</v>
       </c>
       <c r="H31">
         <v>104</v>
@@ -6065,24 +6065,24 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <f t="shared" si="5"/>
-        <v>10.566149988847576</v>
+        <f t="shared" si="0"/>
+        <v>9.1019500424953552</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>10.566149988847576</v>
+        <v>9.1019500424953552</v>
       </c>
       <c r="E32">
         <f t="shared" si="2"/>
-        <v>111.64352558682363</v>
+        <v>82.845494576081194</v>
       </c>
       <c r="F32">
         <f t="shared" si="3"/>
-        <v>111.64352558682363</v>
+        <v>82.845494576081194</v>
       </c>
       <c r="G32">
         <f t="shared" si="4"/>
-        <v>111.64352558682363</v>
+        <v>82.845494576081194</v>
       </c>
       <c r="H32">
         <v>100</v>
@@ -6096,24 +6096,24 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" si="5"/>
-        <v>10.726121000406712</v>
+        <f t="shared" si="0"/>
+        <v>9.2016962093139263</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>11.262427050427048</v>
+        <v>9.6617810197796228</v>
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
-        <v>120.80215530113418</v>
+        <v>88.9047737849274</v>
       </c>
       <c r="F33">
         <f t="shared" si="3"/>
-        <v>115.04967171536589</v>
+        <v>84.671213128502274</v>
       </c>
       <c r="G33">
         <f t="shared" si="4"/>
-        <v>126.8422630661909</v>
+        <v>93.350012474173766</v>
       </c>
       <c r="H33">
         <v>105</v>
@@ -6127,24 +6127,24 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <f t="shared" si="5"/>
-        <v>10.883479980274279</v>
+        <f t="shared" si="0"/>
+        <v>9.2994158084619372</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>11.209984379682508</v>
+        <v>9.5783982827157956</v>
       </c>
       <c r="E34">
         <f t="shared" si="2"/>
-        <v>122.00364057546196</v>
+        <v>89.073508410031934</v>
       </c>
       <c r="F34">
         <f t="shared" si="3"/>
-        <v>118.45013648103102</v>
+        <v>86.479134378671787</v>
       </c>
       <c r="G34">
         <f t="shared" si="4"/>
-        <v>125.66374979272582</v>
+        <v>91.745713662332903</v>
       </c>
       <c r="H34">
         <v>103</v>
@@ -6158,24 +6158,24 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <f t="shared" si="5"/>
-        <v>11.038346848659168</v>
+        <f t="shared" si="0"/>
+        <v>9.3952096054422736</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>11.369497254118944</v>
+        <v>9.6770658936055423</v>
       </c>
       <c r="E35">
         <f t="shared" si="2"/>
-        <v>125.50045418584291</v>
+        <v>90.918062436100612</v>
       </c>
       <c r="F35">
         <f t="shared" si="3"/>
-        <v>121.84510115130379</v>
+        <v>88.269963530194758</v>
       </c>
       <c r="G35">
         <f t="shared" si="4"/>
-        <v>129.2654678114182</v>
+        <v>93.645604309183625</v>
       </c>
       <c r="H35">
         <v>103</v>
@@ -6189,24 +6189,24 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" si="5"/>
-        <v>11.190832679022678</v>
+        <f t="shared" si="0"/>
+        <v>9.4891705645934614</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>11.414649332603132</v>
+        <v>9.6789539758853316</v>
       </c>
       <c r="E36">
         <f t="shared" si="2"/>
-        <v>127.73943077087954</v>
+        <v>91.84524516402594</v>
       </c>
       <c r="F36">
         <f t="shared" si="3"/>
-        <v>125.2347360498819</v>
+        <v>90.044358003946996</v>
       </c>
       <c r="G36">
         <f t="shared" si="4"/>
-        <v>130.29421938629713</v>
+        <v>93.682150067306466</v>
       </c>
       <c r="H36">
         <v>102</v>
@@ -6220,24 +6220,24 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" si="5"/>
-        <v>11.341040583263204</v>
+        <f t="shared" si="0"/>
+        <v>9.5813846569153274</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>11.681271800761101</v>
+        <v>9.8688261966227877</v>
       </c>
       <c r="E37">
         <f t="shared" si="2"/>
-        <v>132.47777755655969</v>
+        <v>94.557019902085628</v>
       </c>
       <c r="F37">
         <f t="shared" si="3"/>
-        <v>128.619201511223</v>
+        <v>91.80293194377245</v>
       </c>
       <c r="G37">
         <f t="shared" si="4"/>
-        <v>136.45211088325649</v>
+        <v>97.393730499148191</v>
       </c>
       <c r="H37">
         <v>103</v>
@@ -6251,24 +6251,24 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <f t="shared" si="5"/>
-        <v>11.489066486343532</v>
+        <f t="shared" si="0"/>
+        <v>9.6719315642912758</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>11.489066486343532</v>
+        <v>9.6719315642912758</v>
       </c>
       <c r="E38">
         <f t="shared" si="2"/>
-        <v>131.99864872762211</v>
+        <v>93.546260184333889</v>
       </c>
       <c r="F38">
         <f t="shared" si="3"/>
-        <v>131.99864872762211</v>
+        <v>93.546260184333889</v>
       </c>
       <c r="G38">
         <f t="shared" si="4"/>
-        <v>131.99864872762211</v>
+        <v>93.546260184333889</v>
       </c>
       <c r="H38">
         <v>100</v>
@@ -6282,24 +6282,24 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <f t="shared" si="5"/>
-        <v>11.634999806768336</v>
+        <f t="shared" si="0"/>
+        <v>9.7608852958162693</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>11.984049800971386</v>
+        <v>10.053711854690757</v>
       </c>
       <c r="E39">
         <f t="shared" si="2"/>
-        <v>139.43441711860419</v>
+        <v>98.133128210824722</v>
       </c>
       <c r="F39">
         <f t="shared" si="3"/>
-        <v>135.37322050349923</v>
+        <v>95.274881758082259</v>
       </c>
       <c r="G39">
         <f t="shared" si="4"/>
-        <v>143.61744963216231</v>
+        <v>101.07712205714947</v>
       </c>
       <c r="H39">
         <v>103</v>
@@ -6313,24 +6313,24 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <f t="shared" si="5"/>
-        <v>11.778924056518717</v>
+        <f t="shared" si="0"/>
+        <v>9.848314729209573</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>12.367870259344652</v>
+        <v>10.340730465670052</v>
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
-        <v>145.68020452569709</v>
+        <v>101.83876815584455</v>
       </c>
       <c r="F40">
         <f t="shared" si="3"/>
-        <v>138.74305192923535</v>
+        <v>96.989303005566228</v>
       </c>
       <c r="G40">
         <f t="shared" si="4"/>
-        <v>152.96421475198196</v>
+        <v>106.93070656363678</v>
       </c>
       <c r="H40">
         <v>105</v>
@@ -6344,24 +6344,24 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <f t="shared" si="5"/>
-        <v>11.92091737178742</v>
+        <f t="shared" si="0"/>
+        <v>9.9342840880931291</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>12.397754066658917</v>
+        <v>10.331655451616856</v>
       </c>
       <c r="E41">
         <f t="shared" si="2"/>
-        <v>147.79260182438242</v>
+        <v>102.63760035665796</v>
       </c>
       <c r="F41">
         <f t="shared" si="3"/>
-        <v>142.10827098498308</v>
+        <v>98.690000342940337</v>
       </c>
       <c r="G41">
         <f t="shared" si="4"/>
-        <v>153.70430589735773</v>
+        <v>106.74310437092429</v>
       </c>
       <c r="H41">
         <v>104</v>
@@ -6375,24 +6375,24 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <f t="shared" si="5"/>
-        <v>12.061052984018335</v>
+        <f t="shared" si="0"/>
+        <v>10.018853364135861</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>11.699221394497785</v>
+        <v>9.7182877632117854</v>
       </c>
       <c r="E42">
         <f t="shared" si="2"/>
-        <v>141.10492911079865</v>
+        <v>97.366100050094772</v>
       </c>
       <c r="F42">
         <f t="shared" si="3"/>
-        <v>145.4689990832976</v>
+        <v>100.37742273205646</v>
       </c>
       <c r="G42">
         <f t="shared" si="4"/>
-        <v>136.87178123747469</v>
+        <v>94.445117048591925</v>
       </c>
       <c r="H42">
         <v>97</v>
@@ -6406,24 +6406,24 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <f t="shared" si="5"/>
-        <v>12.199399639249794</v>
+        <f t="shared" si="0"/>
+        <v>10.102078691613837</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>11.955411646464798</v>
+        <v>9.9000371177815598</v>
       </c>
       <c r="E43">
         <f t="shared" si="2"/>
-        <v>145.84884452696545</v>
+        <v>100.01095401372716</v>
       </c>
       <c r="F43">
         <f t="shared" si="3"/>
-        <v>148.82535155812801</v>
+        <v>102.05199389155833</v>
       </c>
       <c r="G43">
         <f t="shared" si="4"/>
-        <v>142.93186763642612</v>
+        <v>98.010734933452611</v>
       </c>
       <c r="H43">
         <v>98</v>
@@ -6437,30 +6437,30 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <f t="shared" si="5"/>
-        <v>12.336021972525179</v>
+        <f t="shared" si="0"/>
+        <v>10.184012680748173</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>11.719220873898919</v>
+        <v>9.3692916662883192</v>
       </c>
       <c r="E44">
         <f t="shared" si="2"/>
-        <v>144.56856620129281</v>
+        <v>95.416985139108434</v>
       </c>
       <c r="F44">
         <f t="shared" si="3"/>
-        <v>152.17743810662401</v>
+        <v>103.7141142816396</v>
       </c>
       <c r="G44">
         <f t="shared" si="4"/>
-        <v>137.34013789122815</v>
+        <v>87.783626327979746</v>
       </c>
       <c r="H44">
         <v>95</v>
       </c>
       <c r="J44">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
@@ -6468,24 +6468,24 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <f t="shared" si="5"/>
-        <v>12.470980843113404</v>
+        <f t="shared" si="0"/>
+        <v>10.264704715204712</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>11.847431800957732</v>
+        <v>9.7514694794444754</v>
       </c>
       <c r="E45">
         <f t="shared" si="2"/>
-        <v>147.74909502983641</v>
+        <v>100.09595474582854</v>
       </c>
       <c r="F45">
         <f t="shared" si="3"/>
-        <v>155.52536318930152</v>
+        <v>105.36416289034584</v>
       </c>
       <c r="G45">
         <f t="shared" si="4"/>
-        <v>140.36164027834457</v>
+        <v>95.09115700853711</v>
       </c>
       <c r="H45">
         <v>95</v>
@@ -6499,24 +6499,24 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <f t="shared" si="5"/>
-        <v>12.604333635434662</v>
+        <f t="shared" si="0"/>
+        <v>10.344201218330644</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>11.974116953662929</v>
+        <v>9.8269911574141116</v>
       </c>
       <c r="E46">
         <f t="shared" si="2"/>
-        <v>150.92576507368207</v>
+        <v>101.65237390304752</v>
       </c>
       <c r="F46">
         <f t="shared" si="3"/>
-        <v>158.86922639334955</v>
+        <v>107.00249884531318</v>
       </c>
       <c r="G46">
         <f t="shared" si="4"/>
-        <v>143.37947681999796</v>
+        <v>96.569755207895142</v>
       </c>
       <c r="H46">
         <v>95</v>
@@ -6530,30 +6530,30 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <f t="shared" si="5"/>
-        <v>12.736134529880655</v>
+        <f t="shared" si="0"/>
+        <v>10.422545892031014</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>12.099327803386622</v>
+        <v>10.318320433110703</v>
       </c>
       <c r="E47">
         <f t="shared" si="2"/>
-        <v>154.0986666250574</v>
+        <v>107.54316824277763</v>
       </c>
       <c r="F47">
         <f t="shared" si="3"/>
-        <v>162.20912276321832</v>
+        <v>108.62946287149256</v>
       </c>
       <c r="G47">
         <f t="shared" si="4"/>
-        <v>146.39373329380453</v>
+        <v>106.46773656034983</v>
       </c>
       <c r="H47">
         <v>95</v>
       </c>
       <c r="J47">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
@@ -6561,24 +6561,24 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <f t="shared" si="5"/>
-        <v>12.866434747127142</v>
+        <f t="shared" si="0"/>
+        <v>10.499779931627018</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>12.73777039965587</v>
+        <v>10.394782132310747</v>
       </c>
       <c r="E48">
         <f t="shared" si="2"/>
-        <v>163.88969167105986</v>
+        <v>109.14292482647147</v>
       </c>
       <c r="F48">
         <f t="shared" si="3"/>
-        <v>165.54514310208069</v>
+        <v>110.24537861259746</v>
       </c>
       <c r="G48">
         <f t="shared" si="4"/>
-        <v>162.25079475434927</v>
+        <v>108.05149557820675</v>
       </c>
       <c r="H48">
         <v>99</v>
@@ -6592,24 +6592,24 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <f t="shared" si="5"/>
-        <v>12.995282769039722</v>
+        <f t="shared" si="0"/>
+        <v>10.575942219567802</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>12.865329941349325</v>
+        <v>10.470182797372123</v>
       </c>
       <c r="E49">
         <f t="shared" si="2"/>
-        <v>167.18860050482769</v>
+        <v>110.73204829332035</v>
       </c>
       <c r="F49">
         <f t="shared" si="3"/>
-        <v>168.87737424730071</v>
+        <v>111.85055383163672</v>
       </c>
       <c r="G49">
         <f t="shared" si="4"/>
-        <v>165.51671449977943</v>
+        <v>109.62472781038714</v>
       </c>
       <c r="H49">
         <v>99</v>
@@ -6623,24 +6623,24 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <f t="shared" si="5"/>
-        <v>13.122724538854074</v>
+        <f t="shared" si="0"/>
+        <v>10.651069500471698</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>12.59781555729991</v>
+        <v>10.22502672045283</v>
       </c>
       <c r="E50">
         <f t="shared" si="2"/>
-        <v>165.31766334973713</v>
+        <v>108.90747024372328</v>
       </c>
       <c r="F50">
         <f t="shared" si="3"/>
-        <v>172.20589932264286</v>
+        <v>113.44528150387842</v>
       </c>
       <c r="G50">
         <f t="shared" si="4"/>
-        <v>158.70495681574764</v>
+        <v>104.55117143397435</v>
       </c>
       <c r="H50">
         <v>96</v>
@@ -6654,24 +6654,24 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <f t="shared" si="5"/>
-        <v>13.248803642956723</v>
+        <f t="shared" si="0"/>
+        <v>10.725196539638706</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>12.983827570097588</v>
+        <v>10.510692608845931</v>
       </c>
       <c r="E51">
         <f t="shared" si="2"/>
-        <v>172.02018201023085</v>
+        <v>112.72924399760049</v>
       </c>
       <c r="F51">
         <f t="shared" si="3"/>
-        <v>175.53079796962334</v>
+        <v>115.02984081387807</v>
       </c>
       <c r="G51">
         <f t="shared" si="4"/>
-        <v>168.57977837002625</v>
+        <v>110.47465911764847</v>
       </c>
       <c r="H51">
         <v>98</v>
@@ -6685,24 +6685,24 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <f t="shared" si="5"/>
-        <v>13.373561476289998</v>
+        <f t="shared" si="0"/>
+        <v>10.798356266892483</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>12.838619017238397</v>
+        <v>10.366422016216784</v>
       </c>
       <c r="E52">
         <f t="shared" si="2"/>
-        <v>171.69806069770357</v>
+        <v>111.94031814406672</v>
       </c>
       <c r="F52">
         <f t="shared" si="3"/>
-        <v>178.85214656010791</v>
+        <v>116.60449806673617</v>
       </c>
       <c r="G52">
         <f t="shared" si="4"/>
-        <v>164.83013826979541</v>
+        <v>107.46270541830405</v>
       </c>
       <c r="H52">
         <v>96</v>
@@ -6716,24 +6716,24 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <f t="shared" si="5"/>
-        <v>13.497037393147355</v>
+        <f t="shared" si="0"/>
+        <v>10.870579907369168</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>13.497037393147355</v>
+        <v>10.870579907369168</v>
       </c>
       <c r="E53">
         <f t="shared" si="2"/>
-        <v>182.17001839201797</v>
+        <v>118.16950752249826</v>
       </c>
       <c r="F53">
         <f t="shared" si="3"/>
-        <v>182.17001839201797</v>
+        <v>118.16950752249826</v>
       </c>
       <c r="G53">
         <f t="shared" si="4"/>
-        <v>182.17001839201797</v>
+        <v>118.16950752249826</v>
       </c>
       <c r="H53">
         <v>100</v>
@@ -6747,24 +6747,24 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <f t="shared" si="5"/>
-        <v>13.619268844904353</v>
+        <f t="shared" si="0"/>
+        <v>10.94189710066445</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>12.938305402659134</v>
+        <v>10.394802245631228</v>
       </c>
       <c r="E54">
         <f t="shared" si="2"/>
-        <v>176.21025967629322</v>
+        <v>113.73885655345265</v>
       </c>
       <c r="F54">
         <f t="shared" si="3"/>
-        <v>185.48448386978234</v>
+        <v>119.7251121615291</v>
       </c>
       <c r="G54">
         <f t="shared" si="4"/>
-        <v>167.39974669247854</v>
+        <v>108.05191372578001</v>
       </c>
       <c r="H54">
         <v>95</v>
@@ -6778,24 +6778,24 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <f t="shared" si="5"/>
-        <v>13.740291506041386</v>
+        <f t="shared" si="0"/>
+        <v>11.012336009574176</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>13.328082760860143</v>
+        <v>10.68196592928695</v>
       </c>
       <c r="E55">
         <f t="shared" si="2"/>
-        <v>183.13174235086325</v>
+        <v>117.63339805613114</v>
       </c>
       <c r="F55">
         <f t="shared" si="3"/>
-        <v>188.79561067099306</v>
+        <v>121.27154438776408</v>
       </c>
       <c r="G55">
         <f t="shared" si="4"/>
-        <v>177.63779008033734</v>
+        <v>114.1043961144472</v>
       </c>
       <c r="H55">
         <v>97</v>
@@ -6809,24 +6809,24 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <f t="shared" si="5"/>
-        <v>13.860139389650893</v>
+        <f t="shared" si="0"/>
+        <v>11.081923419512202</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>13.444335207961366</v>
+        <v>10.749465716926837</v>
       </c>
       <c r="E56">
         <f t="shared" si="2"/>
-        <v>186.34035998353565</v>
+        <v>119.12475587565504</v>
       </c>
       <c r="F56">
         <f t="shared" si="3"/>
-        <v>192.10346390055224</v>
+        <v>122.80902667593303</v>
       </c>
       <c r="G56">
         <f t="shared" si="4"/>
-        <v>180.7501491840296</v>
+        <v>115.55101319938539</v>
       </c>
       <c r="H56">
         <v>97</v>
@@ -6840,24 +6840,24 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <f t="shared" si="5"/>
-        <v>13.978844953481019</v>
+        <f t="shared" si="0"/>
+        <v>11.150684829558992</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>13.279902705806968</v>
+        <v>10.593150588081041</v>
       </c>
       <c r="E57">
         <f t="shared" si="2"/>
-        <v>185.63770092178868</v>
+        <v>118.12088355974919</v>
       </c>
       <c r="F57">
         <f t="shared" si="3"/>
-        <v>195.40810623346175</v>
+        <v>124.33777216815704</v>
       </c>
       <c r="G57">
         <f t="shared" si="4"/>
-        <v>176.35581587569925</v>
+        <v>112.21483938176171</v>
       </c>
       <c r="H57">
         <v>95</v>
@@ -6871,24 +6871,24 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <f t="shared" si="5"/>
-        <v>14.096439197445546</v>
+        <f t="shared" si="0"/>
+        <v>11.218644535981548</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>13.814510413496635</v>
+        <v>10.994271645261918</v>
       </c>
       <c r="E58">
         <f t="shared" si="2"/>
-        <v>194.73540608633365</v>
+        <v>123.34082552021448</v>
       </c>
       <c r="F58">
         <f t="shared" si="3"/>
-        <v>198.70959804727923</v>
+        <v>125.85798522470866</v>
       </c>
       <c r="G58">
         <f t="shared" si="4"/>
-        <v>190.84069796460696</v>
+        <v>120.87400900981021</v>
       </c>
       <c r="H58">
         <v>98</v>
@@ -6902,24 +6902,24 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <f t="shared" si="5"/>
-        <v>14.212951753423965</v>
+        <f t="shared" si="0"/>
+        <v>11.285825708967824</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>13.502304165752767</v>
+        <v>10.721534423519433</v>
       </c>
       <c r="E59">
         <f t="shared" si="2"/>
-        <v>191.90759766789949</v>
+        <v>121.00136883653913</v>
       </c>
       <c r="F59">
         <f t="shared" si="3"/>
-        <v>202.00799754515737</v>
+        <v>127.36986193319909</v>
       </c>
       <c r="G59">
         <f t="shared" si="4"/>
-        <v>182.31221778450453</v>
+        <v>114.95130039471218</v>
       </c>
       <c r="H59">
         <v>95</v>
@@ -6933,24 +6933,24 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <f t="shared" si="5"/>
-        <v>14.328410968083151</v>
+        <f t="shared" si="0"/>
+        <v>11.35225046323372</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>13.611990419678992</v>
+        <v>10.784637940072033</v>
       </c>
       <c r="E60">
         <f t="shared" si="2"/>
-        <v>195.03819282677125</v>
+        <v>122.42991105099068</v>
       </c>
       <c r="F60">
         <f t="shared" si="3"/>
-        <v>205.30336087028556</v>
+        <v>128.87359057999021</v>
       </c>
       <c r="G60">
         <f t="shared" si="4"/>
-        <v>185.28628318543267</v>
+        <v>116.30841549844114</v>
       </c>
       <c r="H60">
         <v>95</v>
@@ -6964,24 +6964,24 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <f t="shared" si="5"/>
-        <v>14.442843979371592</v>
+        <f t="shared" si="0"/>
+        <v>11.417939923087099</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>13.865130220196727</v>
+        <v>10.961222326163615</v>
       </c>
       <c r="E61">
         <f t="shared" si="2"/>
-        <v>200.25191252397141</v>
+        <v>125.15457800373717</v>
       </c>
       <c r="F61">
         <f t="shared" si="3"/>
-        <v>208.59574221247024</v>
+        <v>130.36935208722622</v>
       </c>
       <c r="G61">
         <f t="shared" si="4"/>
-        <v>192.24183602301255</v>
+        <v>120.14839488358768</v>
       </c>
       <c r="H61">
         <v>96</v>
@@ -6995,24 +6995,24 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <f t="shared" si="5"/>
-        <v>14.556276787266684</v>
+        <f t="shared" si="0"/>
+        <v>11.482914282468647</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>14.410714019394018</v>
+        <v>11.368085139643961</v>
       </c>
       <c r="E62">
         <f t="shared" si="2"/>
-        <v>209.76634196844373</v>
+        <v>130.53874721433723</v>
       </c>
       <c r="F62">
         <f t="shared" si="3"/>
-        <v>211.8851939075189</v>
+        <v>131.85732041852245</v>
       </c>
       <c r="G62">
         <f t="shared" si="4"/>
-        <v>207.66867854875929</v>
+        <v>129.23335974219387</v>
       </c>
       <c r="H62">
         <v>99</v>
@@ -7026,24 +7026,24 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <f t="shared" si="5"/>
-        <v>14.668734319293485</v>
+        <f t="shared" si="0"/>
+        <v>11.547192860432963</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>15.40217103525816</v>
+        <v>12.124552503454611</v>
       </c>
       <c r="E63">
         <f t="shared" si="2"/>
-        <v>225.93035485651944</v>
+        <v>140.00454610383568</v>
       </c>
       <c r="F63">
         <f t="shared" si="3"/>
-        <v>215.17176653001849</v>
+        <v>133.33766295603399</v>
       </c>
       <c r="G63">
         <f t="shared" si="4"/>
-        <v>237.22687259934543</v>
+        <v>147.00477340902748</v>
       </c>
       <c r="H63">
         <v>105</v>
@@ -7057,24 +7057,24 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <f t="shared" si="5"/>
-        <v>14.780240491279267</v>
+        <f t="shared" si="0"/>
+        <v>11.610794152483853</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>15.519252515843231</v>
+        <v>12.191333860108047</v>
       </c>
       <c r="E64">
         <f t="shared" si="2"/>
-        <v>229.37828442905376</v>
+        <v>141.55106789392093</v>
       </c>
       <c r="F64">
         <f t="shared" si="3"/>
-        <v>218.45550898005118</v>
+        <v>134.81054085135324</v>
       </c>
       <c r="G64">
         <f t="shared" si="4"/>
-        <v>240.84719865050647</v>
+        <v>148.62862128861698</v>
       </c>
       <c r="H64">
         <v>105</v>
@@ -7088,24 +7088,24 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <f t="shared" si="5"/>
-        <v>14.89081826376014</v>
+        <f t="shared" si="0"/>
+        <v>11.673735878134163</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>15.486450994310546</v>
+        <v>12.14068531325953</v>
       </c>
       <c r="E65">
         <f t="shared" si="2"/>
-        <v>230.60592730690587</v>
+        <v>141.72715372653428</v>
       </c>
       <c r="F65">
         <f t="shared" si="3"/>
-        <v>221.73646856433257</v>
+        <v>136.27610935243681</v>
       </c>
       <c r="G65">
         <f t="shared" si="4"/>
-        <v>239.83016439918211</v>
+        <v>147.39623987559565</v>
       </c>
       <c r="H65">
         <v>104</v>
@@ -7119,30 +7119,30 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <f t="shared" si="5"/>
-        <v>15.000489694413639</v>
+        <f t="shared" si="0"/>
+        <v>11.736035025022213</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>15.600509282190185</v>
+        <v>11.618674674771992</v>
       </c>
       <c r="E66">
         <f t="shared" si="2"/>
-        <v>234.01527871509819</v>
+        <v>136.35717292746267</v>
       </c>
       <c r="F66">
         <f t="shared" si="3"/>
-        <v>225.01469107220981</v>
+        <v>137.73451810854814</v>
       </c>
       <c r="G66">
         <f t="shared" si="4"/>
-        <v>243.3758898637021</v>
+        <v>134.99360119818803</v>
       </c>
       <c r="H66">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J66">
-        <v>1.04</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.45">
@@ -7150,24 +7150,24 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <f t="shared" si="5"/>
-        <v>15.109275986854044</v>
+        <f t="shared" ref="B67:B89" si="5">2.8*POWER(A67,0.3432946)</f>
+        <v>11.797707889883082</v>
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C89" si="6">B67*J67</f>
-        <v>15.713647026328207</v>
+        <v>12.269616205478405</v>
       </c>
       <c r="E67">
         <f t="shared" si="2"/>
-        <v>237.42182968080124</v>
+        <v>144.75334791320989</v>
       </c>
       <c r="F67">
         <f t="shared" si="3"/>
-        <v>228.29022084692426</v>
+        <v>139.18591145500952</v>
       </c>
       <c r="G67">
         <f t="shared" si="4"/>
-        <v>246.91870286803331</v>
+        <v>150.54348182973828</v>
       </c>
       <c r="H67">
         <v>104</v>
@@ -7182,23 +7182,23 @@
       </c>
       <c r="B68">
         <f t="shared" si="5"/>
-        <v>15.217197536093702</v>
+        <v>11.858770116642992</v>
       </c>
       <c r="C68">
         <f t="shared" si="6"/>
-        <v>15.825885437537449</v>
+        <v>12.333120921308712</v>
       </c>
       <c r="E68">
         <f t="shared" ref="E68:E89" si="7">B68*C68</f>
-        <v>240.82562488659607</v>
+        <v>146.25564582656023</v>
       </c>
       <c r="F68">
         <f t="shared" ref="F68:F89" si="8">B68*B68</f>
-        <v>231.56310085249623</v>
+        <v>140.63042867938483</v>
       </c>
       <c r="G68">
         <f t="shared" ref="G68:G89" si="9">C68*C68</f>
-        <v>250.45864988205992</v>
+        <v>152.10587165962266</v>
       </c>
       <c r="H68">
         <v>104</v>
@@ -7213,23 +7213,23 @@
       </c>
       <c r="B69">
         <f t="shared" si="5"/>
-        <v>15.324273970944441</v>
+        <v>11.919236731878554</v>
       </c>
       <c r="C69">
         <f t="shared" si="6"/>
-        <v>15.784002190072774</v>
+        <v>12.276813833834911</v>
       </c>
       <c r="E69">
         <f t="shared" si="7"/>
-        <v>241.87837391866228</v>
+        <v>146.33025039867985</v>
       </c>
       <c r="F69">
         <f t="shared" si="8"/>
-        <v>234.83337273656531</v>
+        <v>142.06820427056294</v>
       </c>
       <c r="G69">
         <f t="shared" si="9"/>
-        <v>249.13472513622213</v>
+        <v>150.72015791064024</v>
       </c>
       <c r="H69">
         <v>103</v>
@@ -7243,30 +7243,30 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <f t="shared" ref="B70:B89" si="10">2.08*POWER(A70,0.4732946)</f>
-        <v>15.430524193606809</v>
+        <f t="shared" si="5"/>
+        <v>11.97912217785902</v>
       </c>
       <c r="C70">
         <f t="shared" si="6"/>
-        <v>16.202050403287149</v>
+        <v>12.817660730309152</v>
       </c>
       <c r="E70">
         <f t="shared" si="7"/>
-        <v>250.00613073395931</v>
+        <v>153.544323922719</v>
       </c>
       <c r="F70">
         <f t="shared" si="8"/>
-        <v>238.10107688948506</v>
+        <v>143.49936815207383</v>
       </c>
       <c r="G70">
         <f t="shared" si="9"/>
-        <v>262.50643727065727</v>
+        <v>164.29242659730934</v>
       </c>
       <c r="H70">
         <v>105</v>
       </c>
       <c r="J70">
-        <v>1.05</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.45">
@@ -7274,24 +7274,24 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <f t="shared" si="10"/>
-        <v>15.535966416671609</v>
+        <f t="shared" si="5"/>
+        <v>12.038440343368887</v>
       </c>
       <c r="C71">
         <f t="shared" si="6"/>
-        <v>16.157405073338474</v>
+        <v>12.519977957103643</v>
       </c>
       <c r="E71">
         <f t="shared" si="7"/>
-        <v>251.020902599946</v>
+        <v>150.72100773688567</v>
       </c>
       <c r="F71">
         <f t="shared" si="8"/>
-        <v>241.36625249994808</v>
+        <v>144.92404590085161</v>
       </c>
       <c r="G71">
         <f t="shared" si="9"/>
-        <v>261.06173870394383</v>
+        <v>156.74984804636111</v>
       </c>
       <c r="H71">
         <v>104</v>
@@ -7305,24 +7305,24 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <f t="shared" si="10"/>
-        <v>15.64061819773721</v>
+        <f t="shared" si="5"/>
+        <v>12.097204592489296</v>
       </c>
       <c r="C72">
         <f t="shared" si="6"/>
-        <v>16.422649107624071</v>
+        <v>12.702064822113762</v>
       </c>
       <c r="E72">
         <f t="shared" si="7"/>
-        <v>256.86038448775781</v>
+        <v>153.65947690017134</v>
       </c>
       <c r="F72">
         <f t="shared" si="8"/>
-        <v>244.62893760738837</v>
+        <v>146.34235895254412</v>
       </c>
       <c r="G72">
         <f t="shared" si="9"/>
-        <v>269.7034037121457</v>
+        <v>161.34245074517992</v>
       </c>
       <c r="H72">
         <v>105</v>
@@ -7336,24 +7336,24 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <f t="shared" si="10"/>
-        <v>15.744496471827718</v>
+        <f t="shared" si="5"/>
+        <v>12.155427791500214</v>
       </c>
       <c r="C73">
         <f t="shared" si="6"/>
-        <v>16.374276330700827</v>
+        <v>12.641644903160223</v>
       </c>
       <c r="E73">
         <f t="shared" si="7"/>
-        <v>257.8047359174513</v>
+        <v>153.66460178615083</v>
       </c>
       <c r="F73">
         <f t="shared" si="8"/>
-        <v>247.88916915139546</v>
+        <v>147.75442479437578</v>
       </c>
       <c r="G73">
         <f t="shared" si="9"/>
-        <v>268.11692535414932</v>
+        <v>159.81118585759685</v>
       </c>
       <c r="H73">
         <v>104</v>
@@ -7367,24 +7367,24 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <f t="shared" si="10"/>
-        <v>15.84761758178008</v>
+        <f t="shared" si="5"/>
+        <v>12.213122334050334</v>
       </c>
       <c r="C74">
         <f t="shared" si="6"/>
-        <v>16.639998460869084</v>
+        <v>12.823778450752851</v>
       </c>
       <c r="E74">
         <f t="shared" si="7"/>
-        <v>263.70433216926233</v>
+        <v>156.61837500380304</v>
       </c>
       <c r="F74">
         <f t="shared" si="8"/>
-        <v>251.14698301834511</v>
+        <v>149.16035714647907</v>
       </c>
       <c r="G74">
         <f t="shared" si="9"/>
-        <v>276.88954877772545</v>
+        <v>164.4492937539932</v>
       </c>
       <c r="H74">
         <v>105</v>
@@ -7398,24 +7398,24 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <f t="shared" si="10"/>
-        <v>15.949997306753463</v>
+        <f t="shared" si="5"/>
+        <v>12.270300164728402</v>
       </c>
       <c r="C75">
         <f t="shared" si="6"/>
-        <v>16.587997199023601</v>
+        <v>12.761112171317539</v>
       </c>
       <c r="E75">
         <f t="shared" si="7"/>
-        <v>264.5785106488604</v>
+        <v>156.58267677783522</v>
       </c>
       <c r="F75">
         <f t="shared" si="8"/>
-        <v>254.40241408544273</v>
+        <v>150.56026613253385</v>
       </c>
       <c r="G75">
         <f t="shared" si="9"/>
-        <v>275.16165107481481</v>
+        <v>162.84598384894863</v>
       </c>
       <c r="H75">
         <v>104</v>
@@ -7429,29 +7429,30 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <f t="shared" si="10"/>
-        <v>16.051650889000577</v>
+        <f t="shared" si="5"/>
+        <v>12.326972801157565</v>
       </c>
       <c r="C76">
         <f t="shared" si="6"/>
-        <v>16.533200415670596</v>
+        <v>12.696781985192292</v>
       </c>
       <c r="E76">
         <f t="shared" si="7"/>
-        <v>265.38516115022361</v>
+        <v>156.51288619369274</v>
       </c>
       <c r="F76">
         <f t="shared" si="8"/>
-        <v>257.65549626235298</v>
+        <v>151.95425844047838</v>
       </c>
       <c r="G76">
         <f t="shared" si="9"/>
-        <v>273.34671598473034</v>
+        <v>161.20827277950352</v>
       </c>
       <c r="H76">
         <v>103</v>
       </c>
       <c r="J76">
+        <f t="shared" ref="J76:J87" si="10">H76/100</f>
         <v>1.03</v>
       </c>
     </row>
@@ -7460,30 +7461,30 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <f t="shared" si="10"/>
-        <v>16.152593059028717</v>
+        <f t="shared" si="5"/>
+        <v>12.383151354723799</v>
       </c>
       <c r="C77">
         <f t="shared" si="6"/>
-        <v>16.798696781389868</v>
+        <v>12.395534506078521</v>
       </c>
       <c r="E77">
         <f t="shared" si="7"/>
-        <v>271.34251303180605</v>
+        <v>153.49577991147183</v>
       </c>
       <c r="F77">
         <f t="shared" si="8"/>
-        <v>260.90626253058269</v>
+        <v>153.34243747399785</v>
       </c>
       <c r="G77">
         <f t="shared" si="9"/>
-        <v>282.19621355307834</v>
+        <v>153.64927569138328</v>
       </c>
       <c r="H77">
         <v>104</v>
       </c>
       <c r="J77">
-        <v>1.04</v>
+        <v>1.0009999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.45">
@@ -7491,29 +7492,30 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <f t="shared" si="10"/>
-        <v>16.252838059267091</v>
+        <f t="shared" si="5"/>
+        <v>12.438846550039468</v>
       </c>
       <c r="C78">
         <f t="shared" si="6"/>
-        <v>16.740423201045104</v>
+        <v>12.812011946540652</v>
       </c>
       <c r="E78">
         <f t="shared" si="7"/>
-        <v>272.07938733018369</v>
+        <v>159.36665060029165</v>
       </c>
       <c r="F78">
         <f t="shared" si="8"/>
-        <v>264.15474498076088</v>
+        <v>154.72490349542878</v>
       </c>
       <c r="G78">
         <f t="shared" si="9"/>
-        <v>280.24176895008918</v>
+        <v>164.14765011830039</v>
       </c>
       <c r="H78">
         <v>103</v>
       </c>
       <c r="J78">
+        <f t="shared" si="10"/>
         <v>1.03</v>
       </c>
     </row>
@@ -7522,29 +7524,30 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <f t="shared" si="10"/>
-        <v>16.352399666347399</v>
+        <f t="shared" si="5"/>
+        <v>12.494068743234765</v>
       </c>
       <c r="C79">
         <f t="shared" si="6"/>
-        <v>17.333543646328245</v>
+        <v>13.243712867828851</v>
       </c>
       <c r="E79">
         <f t="shared" si="7"/>
-        <v>283.44503333883608</v>
+        <v>165.46785898631649</v>
       </c>
       <c r="F79">
         <f t="shared" si="8"/>
-        <v>267.40097484795854</v>
+        <v>156.10175376067593</v>
       </c>
       <c r="G79">
         <f t="shared" si="9"/>
-        <v>300.45173533916625</v>
+        <v>175.39593052549549</v>
       </c>
       <c r="H79">
         <v>106</v>
       </c>
       <c r="J79">
+        <f t="shared" si="10"/>
         <v>1.06</v>
       </c>
     </row>
@@ -7553,30 +7556,30 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <f t="shared" si="10"/>
-        <v>16.451291212095569</v>
+        <f t="shared" si="5"/>
+        <v>12.548827939161528</v>
       </c>
       <c r="C80">
         <f t="shared" si="6"/>
-        <v>17.438368684821302</v>
+        <v>12.799804497944759</v>
       </c>
       <c r="E80">
         <f t="shared" si="7"/>
-        <v>286.88368149788323</v>
+        <v>160.62254429961459</v>
       </c>
       <c r="F80">
         <f t="shared" si="8"/>
-        <v>270.64498254517292</v>
+        <v>157.47308264668098</v>
       </c>
       <c r="G80">
         <f t="shared" si="9"/>
-        <v>304.09670238775624</v>
+        <v>163.83499518560689</v>
       </c>
       <c r="H80">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J80">
-        <v>1.06</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.45">
@@ -7584,29 +7587,30 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <f t="shared" si="10"/>
-        <v>16.549525603324515</v>
+        <f t="shared" si="5"/>
+        <v>12.603133807587065</v>
       </c>
       <c r="C81">
         <f t="shared" si="6"/>
-        <v>17.542497139523988</v>
+        <v>13.359321836042289</v>
       </c>
       <c r="E81">
         <f t="shared" si="7"/>
-        <v>290.32000555679929</v>
+        <v>168.36932067826069</v>
       </c>
       <c r="F81">
         <f t="shared" si="8"/>
-        <v>273.88679769509366</v>
+        <v>158.83898177194405</v>
       </c>
       <c r="G81">
         <f t="shared" si="9"/>
-        <v>307.7392058902073</v>
+        <v>178.47147991895633</v>
       </c>
       <c r="H81">
         <v>106</v>
       </c>
       <c r="J81">
+        <f t="shared" si="10"/>
         <v>1.06</v>
       </c>
     </row>
@@ -7615,30 +7619,31 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <f t="shared" si="10"/>
-        <v>16.647115340510503</v>
+        <f t="shared" si="5"/>
+        <v>12.656995698449162</v>
       </c>
       <c r="C82">
         <f t="shared" si="6"/>
-        <v>17.645942260941133</v>
+        <v>13.28984548337162</v>
       </c>
       <c r="E82">
         <f t="shared" si="7"/>
-        <v>293.7540361098757</v>
+        <v>168.20951711608862</v>
       </c>
       <c r="F82">
         <f t="shared" si="8"/>
-        <v>277.12644916026011</v>
+        <v>160.19954011056058</v>
       </c>
       <c r="G82">
         <f t="shared" si="9"/>
-        <v>311.37927827646826</v>
+        <v>176.61999297189305</v>
       </c>
       <c r="H82">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J82">
-        <v>1.06</v>
+        <f t="shared" si="10"/>
+        <v>1.05</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.45">
@@ -7646,29 +7651,30 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <f t="shared" si="10"/>
-        <v>16.744072535429062</v>
+        <f t="shared" si="5"/>
+        <v>12.710422656237448</v>
       </c>
       <c r="C83">
         <f t="shared" si="6"/>
-        <v>17.748716887554806</v>
+        <v>13.473048015611695</v>
       </c>
       <c r="E83">
         <f t="shared" si="7"/>
-        <v>297.18580297601244</v>
+        <v>171.24813474620589</v>
       </c>
       <c r="F83">
         <f t="shared" si="8"/>
-        <v>280.3639650717098</v>
+        <v>161.55484410019423</v>
       </c>
       <c r="G83">
         <f t="shared" si="9"/>
-        <v>315.01695115457318</v>
+        <v>181.52302283097825</v>
       </c>
       <c r="H83">
         <v>106</v>
       </c>
       <c r="J83">
+        <f t="shared" si="10"/>
         <v>1.06</v>
       </c>
     </row>
@@ -7677,30 +7683,31 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <f t="shared" si="10"/>
-        <v>16.840408927820356</v>
+        <f t="shared" si="5"/>
+        <v>12.763423433561329</v>
       </c>
       <c r="C84">
         <f t="shared" si="6"/>
-        <v>18.01923755276778</v>
+        <v>13.273960370903783</v>
       </c>
       <c r="E84">
         <f t="shared" si="7"/>
-        <v>303.45132895614637</v>
+        <v>169.42117685415778</v>
       </c>
       <c r="F84">
         <f t="shared" si="8"/>
-        <v>283.59937285621152</v>
+        <v>162.90497774438245</v>
       </c>
       <c r="G84">
         <f t="shared" si="9"/>
-        <v>324.69292198307659</v>
+        <v>176.19802392832409</v>
       </c>
       <c r="H84">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J84">
-        <v>1.07</v>
+        <f t="shared" si="10"/>
+        <v>1.04</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.45">
@@ -7708,30 +7715,30 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <f t="shared" si="10"/>
-        <v>16.936135901148376</v>
+        <f t="shared" si="5"/>
+        <v>12.816006503959533</v>
       </c>
       <c r="C85">
         <f t="shared" si="6"/>
-        <v>17.782942696205794</v>
+        <v>12.687846438919937</v>
       </c>
       <c r="E85">
         <f t="shared" si="7"/>
-        <v>301.17433422527523</v>
+        <v>162.60752248243773</v>
       </c>
       <c r="F85">
         <f t="shared" si="8"/>
-        <v>286.8326992621669</v>
+        <v>164.25002270953306</v>
       </c>
       <c r="G85">
         <f t="shared" si="9"/>
-        <v>316.23305093653897</v>
+        <v>160.98144725761333</v>
       </c>
       <c r="H85">
         <v>105</v>
       </c>
       <c r="J85">
-        <v>1.05</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.45">
@@ -7739,30 +7746,31 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <f t="shared" si="10"/>
-        <v>17.031264497513551</v>
+        <f t="shared" si="5"/>
+        <v>12.868180074002332</v>
       </c>
       <c r="C86">
         <f t="shared" si="6"/>
-        <v>18.223453012339501</v>
+        <v>13.254225476222402</v>
       </c>
       <c r="E86">
         <f t="shared" si="7"/>
-        <v>310.36844831116412</v>
+        <v>170.55776016945919</v>
       </c>
       <c r="F86">
         <f t="shared" si="8"/>
-        <v>290.06397038426547</v>
+        <v>165.59005841695065</v>
       </c>
       <c r="G86">
         <f t="shared" si="9"/>
-        <v>332.09423969294562</v>
+        <v>175.67449297454294</v>
       </c>
       <c r="H86">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J86">
-        <v>1.07</v>
+        <f t="shared" si="10"/>
+        <v>1.03</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.45">
@@ -7770,30 +7778,31 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <f t="shared" si="10"/>
-        <v>17.125805431773422</v>
+        <f t="shared" si="5"/>
+        <v>12.919952094733114</v>
       </c>
       <c r="C87">
         <f t="shared" si="6"/>
-        <v>18.153353757679827</v>
+        <v>13.178351136627777</v>
       </c>
       <c r="E87">
         <f t="shared" si="7"/>
-        <v>310.89080438817763</v>
+        <v>170.26366537280256</v>
       </c>
       <c r="F87">
         <f t="shared" si="8"/>
-        <v>293.29321168696003</v>
+        <v>166.92516213019857</v>
       </c>
       <c r="G87">
         <f t="shared" si="9"/>
-        <v>329.5442526514683</v>
+        <v>173.66893868025861</v>
       </c>
       <c r="H87">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J87">
-        <v>1.06</v>
+        <f t="shared" si="10"/>
+        <v>1.02</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.45">
@@ -7801,30 +7810,31 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <f t="shared" si="10"/>
-        <v>17.219769104922449</v>
+        <f t="shared" si="5"/>
+        <v>12.971330272492855</v>
       </c>
       <c r="C88">
         <f t="shared" si="6"/>
-        <v>18.252955251217795</v>
+        <v>13.101043575217783</v>
       </c>
       <c r="E88">
         <f t="shared" si="7"/>
-        <v>314.31167490845218</v>
+        <v>169.93796312847047</v>
       </c>
       <c r="F88">
         <f t="shared" si="8"/>
-        <v>296.52044802684168</v>
+        <v>168.25540903808957</v>
       </c>
       <c r="G88">
         <f t="shared" si="9"/>
-        <v>333.17037540295928</v>
+        <v>171.63734275975517</v>
       </c>
       <c r="H88">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J88">
-        <v>1.06</v>
+        <f>H88/100</f>
+        <v>1.01</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.45">
@@ -7832,24 +7842,24 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <f t="shared" si="10"/>
-        <v>17.313165616777439</v>
+        <f t="shared" si="5"/>
+        <v>13.022322079167235</v>
       </c>
       <c r="C89">
         <f t="shared" si="6"/>
-        <v>17.313165616777439</v>
+        <v>13.022322079167235</v>
       </c>
       <c r="E89">
         <f t="shared" si="7"/>
-        <v>299.74570367396456</v>
+        <v>169.58087233356648</v>
       </c>
       <c r="F89">
         <f t="shared" si="8"/>
-        <v>299.74570367396456</v>
+        <v>169.58087233356648</v>
       </c>
       <c r="G89">
         <f t="shared" si="9"/>
-        <v>299.74570367396456</v>
+        <v>169.58087233356648</v>
       </c>
       <c r="H89">
         <v>100</v>
@@ -7864,49 +7874,49 @@
       </c>
       <c r="B90">
         <f>SUM(B2:B89)</f>
-        <v>1042.328160997801</v>
+        <v>858.851885043072</v>
       </c>
       <c r="C90">
         <f>SUM(C2:C89)</f>
-        <v>1069.9282228828024</v>
+        <v>877.39335483089985</v>
       </c>
       <c r="E90">
         <f t="shared" ref="E90:G90" si="11">SUM(E2:E89)</f>
-        <v>14040.213360387505</v>
+        <v>9097.2179914900989</v>
       </c>
       <c r="F90">
         <f t="shared" si="11"/>
-        <v>13700.428687196065</v>
+        <v>8931.8304446940947</v>
       </c>
       <c r="G90">
         <f t="shared" si="11"/>
-        <v>14410.465090127213</v>
+        <v>9280.4227387383398</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="F93">
         <f>(88*E90)-(B90*C90)</f>
-        <v>120322.45875702356</v>
+        <v>47004.246530345525</v>
       </c>
       <c r="G93">
         <f>(88*F90)-(B90*B90)</f>
-        <v>119189.72926419601</v>
+        <v>48374.518691042205</v>
       </c>
       <c r="H93">
         <f>(88*G90)-(C90*C90)</f>
-        <v>123374.52581004286</v>
+        <v>46858.101907552569</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H95">
         <f>G93*H93</f>
-        <v>14704976329.397572</v>
+        <v>2266738126.5536623</v>
       </c>
     </row>
     <row r="97" spans="8:8" x14ac:dyDescent="0.45">
       <c r="H97">
         <f>F93/SQRT(H95)</f>
-        <v>0.99223497924983128</v>
+        <v>0.98727109177853012</v>
       </c>
     </row>
   </sheetData>
@@ -7920,7 +7930,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8148,10 +8158,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF530640-CAD9-4574-9A82-A4E971A6AB3C}">
-  <dimension ref="B1:O11"/>
+  <dimension ref="B1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8178,7 +8188,7 @@
       </c>
       <c r="H1" s="4">
         <f>O1/D1*100</f>
-        <v>22.735598595240589</v>
+        <v>15.829751546283678</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>11</v>
@@ -8187,7 +8197,7 @@
         <v>25.38</v>
       </c>
       <c r="O1" s="3">
-        <v>17.349989999999998</v>
+        <v>12.08</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.45">
@@ -8204,15 +8214,15 @@
         <v>10</v>
       </c>
       <c r="F2" s="4">
-        <f t="shared" ref="F2:F10" si="0">N2/D2*100</f>
+        <f t="shared" ref="F2:F6" si="0">N2/D2*100</f>
         <v>59.337044534412954</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="4">
-        <f t="shared" ref="H2:H10" si="1">O2/D2*100</f>
-        <v>26.295151189271255</v>
+        <f t="shared" ref="H2:H6" si="1">O2/D2*100</f>
+        <v>18.028846153846153</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
@@ -8221,7 +8231,7 @@
         <v>37.520000000000003</v>
       </c>
       <c r="O2" s="3">
-        <v>16.626950000000001</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.45">
@@ -8246,7 +8256,7 @@
       </c>
       <c r="H3" s="4">
         <f t="shared" si="1"/>
-        <v>30.220733610822066</v>
+        <v>21.765998959417274</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>11</v>
@@ -8255,7 +8265,7 @@
         <v>46.474440000000001</v>
       </c>
       <c r="O3" s="3">
-        <v>18.586960000000001</v>
+        <v>13.38696</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.45">
@@ -8279,8 +8289,8 @@
         <v>10</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="1"/>
-        <v>32.512121212121215</v>
+        <f>O4/D4*100</f>
+        <v>20.160342555994731</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>11</v>
@@ -8289,7 +8299,7 @@
         <v>73.15064000000001</v>
       </c>
       <c r="O4" s="3">
-        <v>19.74136</v>
+        <v>12.24136</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.45">
@@ -8314,7 +8324,7 @@
       </c>
       <c r="H5" s="4">
         <f t="shared" si="1"/>
-        <v>33.724174385823595</v>
+        <v>25.221506242448648</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>11</v>
@@ -8323,7 +8333,7 @@
         <v>34.92</v>
       </c>
       <c r="O5" s="3">
-        <v>20.096910000000001</v>
+        <v>15.03</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.45">
@@ -8348,7 +8358,7 @@
       </c>
       <c r="H6" s="4">
         <f t="shared" si="1"/>
-        <v>37.274542754416132</v>
+        <v>27.317492574644366</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>11</v>
@@ -8357,88 +8367,52 @@
         <v>50.395519999999998</v>
       </c>
       <c r="O6" s="3">
-        <v>19.075620000000001</v>
+        <v>13.98</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="2"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="2"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="2"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="2"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4">
-        <f>SUM(D1:D10)/10</f>
-        <v>37.253599999999999</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D7" s="4">
+        <f>SUM(D1:D6)/6</f>
+        <v>62.089333333333336</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4">
-        <f t="shared" ref="E11:F11" si="2">SUM(F1:F10)/10</f>
-        <v>44.57039763559569</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F7" s="4">
+        <f>SUM(F1:F6)/6</f>
+        <v>74.283996059326157</v>
+      </c>
+      <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="4">
-        <f t="shared" ref="H11" si="3">SUM(H1:H10)/10</f>
-        <v>18.276232174769483</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="H7" s="4">
+        <f>SUM(H1:H6)/6</f>
+        <v>21.387323005439143</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N7" s="3">
         <v>50.921964000000003</v>
       </c>
-      <c r="O11" s="3">
-        <f>AVERAGE(O1:O10)</f>
-        <v>18.579631666666668</v>
+      <c r="O7" s="3">
+        <f>AVERAGE(O1:O6)</f>
+        <v>13.01972</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:G10">
-    <sortCondition descending="1" ref="D1:D10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:G6">
+    <sortCondition descending="1" ref="D1:D6"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="I1" r:id="rId1" xr:uid="{F521CDC8-1FC7-476D-BFC6-77EC50008475}"/>
-    <hyperlink ref="I2:I11" r:id="rId2" display="\\" xr:uid="{C9C6E8C5-9CF6-4DFC-9F6B-537553C5EF8E}"/>
+    <hyperlink ref="I2:I7" r:id="rId2" display="\\" xr:uid="{C9C6E8C5-9CF6-4DFC-9F6B-537553C5EF8E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>

</xml_diff>

<commit_message>
update figures and tables, conclusion and references
added pictures, re structured some chaptertitles
</commit_message>
<xml_diff>
--- a/thesis/graphs/wpm.xlsx
+++ b/thesis/graphs/wpm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samii\Documents\mtd\thesis\thesisType\thesis\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554C56C0-6ABF-483C-A99C-4D64B429C2BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18BEEFF-72C5-41CA-963B-BA877282C4C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="1" xr2:uid="{5BCCB96D-E4D3-4CE0-AFF7-989508396116}"/>
   </bookViews>
@@ -5070,8 +5070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BFA5080-83A4-48B0-9E86-96BE7C4E1BDB}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7894,6 +7894,13 @@
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B93">
+        <v>250</v>
+      </c>
+      <c r="C93">
+        <f t="shared" ref="C93" si="12">2.8*POWER(B93,0.3432946)</f>
+        <v>18.636222523363884</v>
+      </c>
       <c r="F93">
         <f>(88*E90)-(B90*C90)</f>
         <v>47004.246530345525</v>

</xml_diff>